<commit_message>
Atualização planilha de custo
</commit_message>
<xml_diff>
--- a/Custos para Edição.xlsx
+++ b/Custos para Edição.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cássio\Documents\SENAC\PROJETO_INTTEGRADOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Publica\TI0320\Cassio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170B25BC-6AA1-4B30-AB70-4381E41DBDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376D7760-00CA-4850-A8C9-9BEAC1E0241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orçamento de Empresa" sheetId="1" r:id="rId1"/>
@@ -55,8 +55,36 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={423E396C-BC7A-4789-AFE6-1C43DEF629DD}</author>
+    <author>tc={4F5185A9-8010-4F61-810B-0777DA2DE50F}</author>
+  </authors>
+  <commentList>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{423E396C-BC7A-4789-AFE6-1C43DEF629DD}">
+      <text>
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
+    é um instrumento que integra capital e trabalho, tendo como principal objetivo o aumento da produtividade de forma que, nesta situação, a remuneração dos funcionários varia conforme o alcance das metas da organização.</t>
+      </text>
+    </comment>
+    <comment ref="C34" authorId="1" shapeId="0" xr:uid="{4F5185A9-8010-4F61-810B-0777DA2DE50F}">
+      <text>
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
+    Nesse custo, foi feito um contrato com as montadoras para arcar com 50% do custo.
+O valor que está demonstrado é a metade que a empresa tem que arcar</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>Crie um Orçamento de casamento nesta planilha. Atualize o resumo e o gráfico na planilha atual inserindo detalhes nas tabelas das planilhas Roupas-Festa-Música-Fotos e Decor-Flores-Presentes-Viagem. Instruções úteis sobre como usar esta planilha estão nas células desta coluna. O rótulo Data do casamento está na célula C1.</t>
   </si>
@@ -116,30 +144,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Insira os detalhes na tabela Roupas, começando na célula à direita. A próxima instrução está na célula A18.</t>
-  </si>
-  <si>
-    <t>Gerência de Desenvolvimento</t>
-  </si>
-  <si>
-    <t>Gerência Operacional</t>
-  </si>
-  <si>
-    <t>Supervisores de Planejamento (2)²</t>
-  </si>
-  <si>
-    <t>Time de Planejamento (8)</t>
-  </si>
-  <si>
-    <t>Supervisor de Desenvolvimento</t>
-  </si>
-  <si>
-    <t>Time de Desenvolvimento (7)</t>
-  </si>
-  <si>
-    <t>Supervisor de Operacional (5)</t>
-  </si>
-  <si>
-    <t>Time de Operacional (50)</t>
   </si>
   <si>
     <t>Total de Custo¹</t>
@@ -172,9 +176,6 @@
     <t>Insira na tabela que começa na célula à direita os custos com a Festa, excluindo os custos com Entretenimento e Decoração. A próxima instrução está na célula A31.</t>
   </si>
   <si>
-    <t>Escritório</t>
-  </si>
-  <si>
     <t>Luz</t>
   </si>
   <si>
@@ -187,9 +188,6 @@
     <t>Insumos para o Escritório</t>
   </si>
   <si>
-    <t>Galpão</t>
-  </si>
-  <si>
     <t>Periféricos Escritório / Galpão</t>
   </si>
   <si>
@@ -229,15 +227,9 @@
     <t>Show Room</t>
   </si>
   <si>
-    <t>Comerciais Radio/Televisão</t>
-  </si>
-  <si>
     <t>Brindes Personalizados</t>
   </si>
   <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Patrocínios</t>
   </si>
   <si>
@@ -247,12 +239,6 @@
     <t>CFO (Cássio)</t>
   </si>
   <si>
-    <t>A definir (Djeniffer)</t>
-  </si>
-  <si>
-    <t>A definir (Aryon)</t>
-  </si>
-  <si>
     <t>A definir (Maxwell)</t>
   </si>
   <si>
@@ -268,9 +254,6 @@
     <t>Gastos com Veículos</t>
   </si>
   <si>
-    <t>Carro</t>
-  </si>
-  <si>
     <t>Seguro do carro</t>
   </si>
   <si>
@@ -280,7 +263,46 @@
     <t>Seguro patrimonial</t>
   </si>
   <si>
-    <t>uigi</t>
+    <t>Carro (Translado)</t>
+  </si>
+  <si>
+    <t>Galpão / Escritório</t>
+  </si>
+  <si>
+    <t>CCO (Djeniffer)</t>
+  </si>
+  <si>
+    <t>CTO (Aryon)</t>
+  </si>
+  <si>
+    <t>Equipe do Desenvolvimento (3)</t>
+  </si>
+  <si>
+    <t>Equipe Financeiro (2)</t>
+  </si>
+  <si>
+    <t>Equipe Operacional (2)</t>
+  </si>
+  <si>
+    <t>PPR</t>
+  </si>
+  <si>
+    <t>Equipe de Comercial (3)</t>
+  </si>
+  <si>
+    <t>Equipe de Marketing (3)</t>
+  </si>
+  <si>
+    <t>Ganhos com a Venda</t>
+  </si>
+  <si>
+    <t>Estimativa de vendas</t>
+  </si>
+  <si>
+    <t>ganho da empresa 8%</t>
+  </si>
+  <si>
+    <t>Total de Ganho</t>
   </si>
 </sst>
 </file>
@@ -295,7 +317,7 @@
     <numFmt numFmtId="166" formatCode="[$-416]d\-mmm\-yy;@"/>
     <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Cambria"/>
@@ -546,6 +568,27 @@
       <name val="Cambria"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.5"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="37">
@@ -968,7 +1011,7 @@
     <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1088,6 +1131,9 @@
     </xf>
     <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1113,10 +1159,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1169,88 +1240,7 @@
     <cellStyle name="Total" xfId="5" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="8" builtinId="3" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="55">
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1277,10 +1267,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1301,6 +1287,148 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1595,15 +1723,15 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Orçamento de casamento" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Orçamento de casamento" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="45"/>
-      <tableStyleElement type="headerRow" dxfId="44"/>
-      <tableStyleElement type="totalRow" dxfId="43"/>
-      <tableStyleElement type="lastColumn" dxfId="42"/>
+      <tableStyleElement type="wholeTable" dxfId="54"/>
+      <tableStyleElement type="headerRow" dxfId="53"/>
+      <tableStyleElement type="totalRow" dxfId="52"/>
+      <tableStyleElement type="lastColumn" dxfId="51"/>
     </tableStyle>
     <tableStyle name="Resumo do orçamento de casamento" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="41"/>
-      <tableStyleElement type="headerRow" dxfId="40"/>
-      <tableStyleElement type="totalRow" dxfId="39"/>
+      <tableStyleElement type="wholeTable" dxfId="50"/>
+      <tableStyleElement type="headerRow" dxfId="49"/>
+      <tableStyleElement type="totalRow" dxfId="48"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2561,14 +2689,20 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="CASSIO RODRIGUES BRAGA" id="{97E87E9D-ECF8-4E35-9889-A515C6A71A37}" userId="S::cassio.rbraga@senacsp.edu.br::70b205e4-ccb9-441b-9d8f-e0b6bc17dbf1" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ResumoDoOrçamento" displayName="ResumoDoOrçamento" ref="C6:F11" totalsRowCount="1" headerRowDxfId="38" totalsRowCellStyle="Total">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ResumoDoOrçamento" displayName="ResumoDoOrçamento" ref="C6:F11" totalsRowCount="1" headerRowDxfId="47" totalsRowCellStyle="Total">
   <autoFilter ref="C6:F10" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CATEGORIA" totalsRowLabel="Total de despesas" totalsRowDxfId="37" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CATEGORIA" totalsRowLabel="Total de despesas" totalsRowDxfId="46" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40">
       <calculatedColumnFormula>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2582,18 +2716,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Roupas" displayName="Roupas" ref="B2:E17" totalsRowCount="1">
-  <autoFilter ref="B2:E16" xr:uid="{00000000-0009-0000-0100-00000C000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Roupas" displayName="Roupas" ref="B2:E15" totalsRowCount="1">
+  <autoFilter ref="B2:E14" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Custo¹" dataDxfId="30" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ESTIMADO ANUAL" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Custo¹" dataDxfId="39" totalsRowDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ESTIMADO ANUAL" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="13">
       <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C3-'Funcionários-Local-Extras-Marke'!$D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2607,19 +2741,19 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Festa" displayName="Festa" ref="B22:E31" totalsRowCount="1">
-  <autoFilter ref="B22:E30" xr:uid="{00000000-0009-0000-0100-00000D000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Festa" displayName="Festa" ref="B20:E28" totalsRowCount="1">
+  <autoFilter ref="B20:E27" xr:uid="{00000000-0009-0000-0100-00000D000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Custo" dataDxfId="26" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="ESTIMADO ANUAL" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="0">
-      <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C23-'Funcionários-Local-Extras-Marke'!$D23</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Custo" dataDxfId="35" totalsRowDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="ESTIMADO ANUAL" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="21">
+      <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C21-'Funcionários-Local-Extras-Marke'!$D21</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Orçamento de casamento" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2632,19 +2766,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Música" displayName="Música" ref="B35:E39" totalsRowCount="1" totalsRowDxfId="22">
-  <autoFilter ref="B35:E38" xr:uid="{00000000-0009-0000-0100-00000E000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Música" displayName="Música" ref="B32:E36" totalsRowCount="1" totalsRowDxfId="31">
+  <autoFilter ref="B32:E35" xr:uid="{00000000-0009-0000-0100-00000E000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Gastos Extras" dataDxfId="21" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="4">
-      <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C36-'Funcionários-Local-Extras-Marke'!$D36</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Gastos Extras" dataDxfId="30" totalsRowDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="17">
+      <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C33-'Funcionários-Local-Extras-Marke'!$D33</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Orçamento de casamento" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2657,19 +2791,41 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Impressão" displayName="Impressão" ref="B42:E52" totalsRowCount="1" totalsRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Impressão" displayName="Impressão" ref="B39:E47" totalsRowCount="1" totalsRowDxfId="26">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Marketing" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="ESTIMADO" totalsRowFunction="sum" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" totalsRowDxfId="12">
-      <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C43-'Funcionários-Local-Extras-Marke'!$D43</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Marketing" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="ESTIMADO" totalsRowFunction="sum" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" totalsRowDxfId="4">
+      <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C40-'Funcionários-Local-Extras-Marke'!$D40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Orçamento de casamento" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
       <x14:table altTextSummary="Insira o item da Categoria e os Custos reais e estimados com Impressão e Gráfica nesta tabela. Os Valores Acima ou Abaixo e o Total são calculados automaticamente, e o ícone é atualizado"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{542CD9DA-BE67-4476-B3ED-94AAA93D6D50}" name="Música2" displayName="Música2" ref="B51:E54" totalsRowCount="1" totalsRowDxfId="12">
+  <autoFilter ref="B51:E53" xr:uid="{542CD9DA-BE67-4476-B3ED-94AAA93D6D50}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F828AF69-2C3D-4F7C-BAEB-AE441072E02C}" name="CATEGORIA" totalsRowLabel="Total de Ganho" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{49218F16-1EAB-4FE3-85CD-202EE002DE31}" name="ESTIMADO" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="2">
+      <totalsRowFormula>C53</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{B924C15A-4FC9-4943-9D4C-3A0A2C03CA14}" name="REAL" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{6A452F63-ECF6-47C3-9821-65724FEBC5DB}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0">
+      <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C52-'Funcionários-Local-Extras-Marke'!$D52</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Orçamento de casamento" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Insira o item da Categoria e os Custos reais e estimados com Música e Entretenimento nesta tabela. Os Valores Acima ou Abaixo e o Total são calculados automaticamente, e o ícone é atualizado"/>
     </ext>
   </extLst>
 </table>
@@ -2936,6 +3092,18 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B14" dT="2022-04-01T23:19:19.92" personId="{97E87E9D-ECF8-4E35-9889-A515C6A71A37}" id="{423E396C-BC7A-4789-AFE6-1C43DEF629DD}">
+    <text>é um instrumento que integra capital e trabalho, tendo como principal objetivo o aumento da produtividade de forma que, nesta situação, a remuneração dos funcionários varia conforme o alcance das metas da organização.</text>
+  </threadedComment>
+  <threadedComment ref="C34" dT="2022-04-01T23:22:43.00" personId="{97E87E9D-ECF8-4E35-9889-A515C6A71A37}" id="{4F5185A9-8010-4F61-810B-0777DA2DE50F}">
+    <text>Nesse custo, foi feito um contrato com as montadoras para arcar com 50% do custo.
+O valor que está demonstrado é a metade que a empresa tem que arcar</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
@@ -2944,7 +3112,7 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="50" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -2989,30 +3157,30 @@
         <v>3</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3042,7 +3210,7 @@
       </c>
       <c r="D7" s="49">
         <f>Total_de_Roupas_est</f>
-        <v>750000</v>
+        <v>1218000</v>
       </c>
       <c r="E7" s="49">
         <f>Total_de_Roupas_real</f>
@@ -3050,7 +3218,7 @@
       </c>
       <c r="F7" s="45">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
-        <v>750000</v>
+        <v>1218000</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -3061,7 +3229,7 @@
       </c>
       <c r="D8" s="49">
         <f>Total_da_Festa_est</f>
-        <v>87900</v>
+        <v>67900</v>
       </c>
       <c r="E8" s="49">
         <f>Total_da_Festa_real</f>
@@ -3069,7 +3237,7 @@
       </c>
       <c r="F8" s="45">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
-        <v>87900</v>
+        <v>67900</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -3080,7 +3248,7 @@
       </c>
       <c r="D9" s="49">
         <f>Total_de_Música_entretenimento_est</f>
-        <v>0</v>
+        <v>312500</v>
       </c>
       <c r="E9" s="49">
         <f>Total_de_Música_entretenimento_real</f>
@@ -3088,7 +3256,7 @@
       </c>
       <c r="F9" s="45">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
-        <v>0</v>
+        <v>312500</v>
       </c>
       <c r="G9" s="3"/>
     </row>
@@ -3099,7 +3267,7 @@
       </c>
       <c r="D10" s="49">
         <f>Total_de_Impressão_gráfica_est</f>
-        <v>0</v>
+        <v>120800</v>
       </c>
       <c r="E10" s="49">
         <f>Total_de_Impressão_gráfica_real</f>
@@ -3107,7 +3275,7 @@
       </c>
       <c r="F10" s="45">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
-        <v>0</v>
+        <v>120800</v>
       </c>
       <c r="G10" s="3"/>
     </row>
@@ -3118,7 +3286,7 @@
       </c>
       <c r="D11" s="50">
         <f>SUBTOTAL(109,ResumoDoOrçamento[ESTIMADO])</f>
-        <v>837900</v>
+        <v>1719200</v>
       </c>
       <c r="E11" s="51">
         <f>SUBTOTAL(109,ResumoDoOrçamento[REAL])</f>
@@ -3126,7 +3294,7 @@
       </c>
       <c r="F11" s="47">
         <f>SUBTOTAL(109,ResumoDoOrçamento[ACIMA/ABAIXO])</f>
-        <v>837900</v>
+        <v>1719200</v>
       </c>
       <c r="G11" s="20"/>
     </row>
@@ -3143,204 +3311,204 @@
         <v>15</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
       <c r="G21" s="21"/>
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
       <c r="G29" s="21"/>
     </row>
     <row r="30" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3402,15 +3570,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3419,6 +3587,10 @@
     <col min="2" max="2" width="29.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3442,13 +3614,13 @@
       <c r="B2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="72" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
@@ -3457,7 +3629,7 @@
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="31">
         <v>120000</v>
@@ -3472,7 +3644,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="30" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C4" s="31">
         <v>120000</v>
@@ -3487,7 +3659,7 @@
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="30" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C5" s="31">
         <v>120000</v>
@@ -3502,7 +3674,7 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="31">
         <v>120000</v>
@@ -3517,7 +3689,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="30" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C7" s="31">
         <v>120000</v>
@@ -3531,8 +3703,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
-        <v>62</v>
+      <c r="B8" s="70" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="31">
         <v>150000</v>
@@ -3547,82 +3719,85 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="30" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C9" s="31">
-        <v>0</v>
+        <v>108000</v>
       </c>
       <c r="D9" s="31">
         <v>0</v>
       </c>
       <c r="E9" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C9-'Funcionários-Local-Extras-Marke'!$D9</f>
-        <v>0</v>
+        <v>108000</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="30" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C10" s="31">
-        <v>0</v>
+        <v>108000</v>
       </c>
       <c r="D10" s="31">
         <v>0</v>
       </c>
       <c r="E10" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C10-'Funcionários-Local-Extras-Marke'!$D10</f>
-        <v>0</v>
+        <v>108000</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="30" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C11" s="31">
-        <v>0</v>
+        <v>108000</v>
       </c>
       <c r="D11" s="31">
         <v>0</v>
       </c>
       <c r="E11" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C11-'Funcionários-Local-Extras-Marke'!$D11</f>
-        <v>0</v>
+        <v>108000</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
       <c r="B12" s="30" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C12" s="31">
-        <v>0</v>
+        <v>72000</v>
       </c>
       <c r="D12" s="31">
         <v>0</v>
       </c>
       <c r="E12" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C12-'Funcionários-Local-Extras-Marke'!$D12</f>
-        <v>0</v>
+        <v>72000</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
       <c r="B13" s="30" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C13" s="31">
-        <v>0</v>
+        <v>72000</v>
       </c>
       <c r="D13" s="31">
         <v>0</v>
       </c>
       <c r="E13" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C13-'Funcionários-Local-Extras-Marke'!$D13</f>
-        <v>0</v>
+        <v>72000</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="30" t="s">
-        <v>25</v>
+      <c r="A14" s="16"/>
+      <c r="B14" s="70" t="s">
+        <v>62</v>
       </c>
       <c r="C14" s="31">
         <v>0</v>
@@ -3636,169 +3811,168 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="31">
-        <v>0</v>
-      </c>
-      <c r="D15" s="31">
-        <v>0</v>
-      </c>
-      <c r="E15" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C15-'Funcionários-Local-Extras-Marke'!$D15</f>
-        <v>0</v>
+      <c r="A15" s="15"/>
+      <c r="B15" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="33">
+        <f>SUBTOTAL(109,Roupas[ESTIMADO ANUAL])</f>
+        <v>1218000</v>
+      </c>
+      <c r="D15" s="33">
+        <f>SUBTOTAL(109,Roupas[REAL])</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="34">
+        <f>SUBTOTAL(109,Roupas[ACIMA/ABAIXO])</f>
+        <v>1218000</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="31">
-        <v>0</v>
-      </c>
-      <c r="D16" s="31">
-        <v>0</v>
-      </c>
-      <c r="E16" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C16-'Funcionários-Local-Extras-Marke'!$D16</f>
-        <v>0</v>
-      </c>
+      <c r="A16" s="15"/>
+      <c r="B16" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
-      <c r="B17" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="33">
-        <f>SUBTOTAL(109,Roupas[ESTIMADO ANUAL])</f>
-        <v>750000</v>
-      </c>
-      <c r="D17" s="33">
-        <f>SUBTOTAL(109,Roupas[REAL])</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="34">
-        <f>SUBTOTAL(109,Roupas[ACIMA/ABAIXO])</f>
-        <v>750000</v>
-      </c>
+      <c r="B17" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="57"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
-      <c r="B18" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="59"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
+      <c r="A19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
+      <c r="A20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="36"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="31">
+        <v>3000</v>
+      </c>
+      <c r="D21" s="31">
+        <v>0</v>
+      </c>
+      <c r="E21" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C21-'Funcionários-Local-Extras-Marke'!$D21</f>
+        <v>3000</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>9</v>
+      <c r="B22" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="31">
+        <v>1500</v>
+      </c>
+      <c r="D22" s="31">
+        <v>0</v>
+      </c>
+      <c r="E22" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C22-'Funcionários-Local-Extras-Marke'!$D22</f>
+        <v>1500</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C23" s="31">
-        <v>30000</v>
+        <v>2400</v>
       </c>
       <c r="D23" s="31">
         <v>0</v>
       </c>
       <c r="E23" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C23-'Funcionários-Local-Extras-Marke'!$D23</f>
-        <v>30000</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C24" s="31">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="D24" s="31">
         <v>0</v>
       </c>
       <c r="E24" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C24-'Funcionários-Local-Extras-Marke'!$D24</f>
-        <v>3000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="30" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C25" s="31">
-        <v>1500</v>
+        <v>60000</v>
       </c>
       <c r="D25" s="31">
         <v>0</v>
       </c>
       <c r="E25" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C25-'Funcionários-Local-Extras-Marke'!$D25</f>
-        <v>1500</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="30" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C26" s="31">
-        <v>2400</v>
+        <v>0</v>
       </c>
       <c r="D26" s="31">
         <v>0</v>
       </c>
       <c r="E26" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C26-'Funcionários-Local-Extras-Marke'!$D26</f>
-        <v>2400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="30" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C27" s="31">
         <v>500</v>
@@ -3812,362 +3986,388 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="30" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="33">
+        <f>SUBTOTAL(109,Festa[ESTIMADO ANUAL])</f>
+        <v>67900</v>
+      </c>
+      <c r="D28" s="33">
+        <f>SUBTOTAL(109,Festa[REAL])</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="34">
+        <f>SUBTOTAL(109,Festa[ACIMA/ABAIXO])</f>
+        <v>67900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="57"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="61"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="63"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="36"/>
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="31">
+        <v>0</v>
+      </c>
+      <c r="D33" s="31">
+        <v>0</v>
+      </c>
+      <c r="E33" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C33-'Funcionários-Local-Extras-Marke'!$D33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="67">
+        <f>625000/2</f>
+        <v>312500</v>
+      </c>
+      <c r="D34" s="31">
+        <v>0</v>
+      </c>
+      <c r="E34" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C34-'Funcionários-Local-Extras-Marke'!$D34</f>
+        <v>312500</v>
+      </c>
+      <c r="G34" s="68">
+        <v>130000</v>
+      </c>
+      <c r="H34" s="68">
+        <v>45000</v>
+      </c>
+      <c r="I34" s="68">
+        <v>440000</v>
+      </c>
+      <c r="J34" s="69">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="31">
+        <v>0</v>
+      </c>
+      <c r="D35" s="31">
+        <v>0</v>
+      </c>
+      <c r="E35" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C35-'Funcionários-Local-Extras-Marke'!$D35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="33">
+        <f>SUBTOTAL(109,Música[ESTIMADO])</f>
+        <v>312500</v>
+      </c>
+      <c r="D36" s="33">
+        <f>SUBTOTAL(109,Música[REAL])</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="34">
+        <f>SUBTOTAL(109,Música[ACIMA/ABAIXO])</f>
+        <v>312500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="64"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="66"/>
+    </row>
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="E38" s="29"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="67">
+        <v>5000</v>
+      </c>
+      <c r="D40" s="31">
+        <v>0</v>
+      </c>
+      <c r="E40" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C40-'Funcionários-Local-Extras-Marke'!$D40</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="31">
-        <v>50000</v>
-      </c>
-      <c r="D28" s="31">
-        <v>0</v>
-      </c>
-      <c r="E28" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C28-'Funcionários-Local-Extras-Marke'!$D28</f>
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="31">
-        <v>0</v>
-      </c>
-      <c r="E29" s="32" t="e">
-        <f>'Funcionários-Local-Extras-Marke'!$C29-'Funcionários-Local-Extras-Marke'!$D29</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="30" t="s">
+      <c r="C41" s="31">
+        <v>5000</v>
+      </c>
+      <c r="D41" s="31">
+        <v>0</v>
+      </c>
+      <c r="E41" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C41-'Funcionários-Local-Extras-Marke'!$D41</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="31">
-        <v>500</v>
-      </c>
-      <c r="D30" s="31">
-        <v>0</v>
-      </c>
-      <c r="E30" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C30-'Funcionários-Local-Extras-Marke'!$D30</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="28" t="s">
+      <c r="C42" s="31">
+        <v>5000</v>
+      </c>
+      <c r="D42" s="31">
+        <v>0</v>
+      </c>
+      <c r="E42" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C42-'Funcionários-Local-Extras-Marke'!$D42</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="33">
-        <f>SUBTOTAL(109,Festa[ESTIMADO ANUAL])</f>
-        <v>87900</v>
-      </c>
-      <c r="D31" s="33">
-        <f>SUBTOTAL(109,Festa[REAL])</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="34" t="e">
-        <f>SUBTOTAL(109,Festa[ACIMA/ABAIXO])</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
-    </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="62"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="36"/>
-      <c r="E34" s="29"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="31">
-        <v>0</v>
-      </c>
-      <c r="D36" s="31">
-        <v>0</v>
-      </c>
-      <c r="E36" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C36-'Funcionários-Local-Extras-Marke'!$D36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="31">
-        <v>0</v>
-      </c>
-      <c r="D37" s="31">
-        <v>0</v>
-      </c>
-      <c r="E37" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C37-'Funcionários-Local-Extras-Marke'!$D37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C38-'Funcionários-Local-Extras-Marke'!$D38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="33">
-        <f>SUBTOTAL(109,Música[ESTIMADO])</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="33">
-        <f>SUBTOTAL(109,Música[REAL])</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="34">
-        <f>SUBTOTAL(109,Música[ACIMA/ABAIXO])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="63"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="65"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="36"/>
-      <c r="E41" s="29"/>
-    </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="67">
-        <v>0</v>
+      <c r="C43" s="31">
+        <v>800</v>
       </c>
       <c r="D43" s="31">
         <v>0</v>
       </c>
       <c r="E43" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C43-'Funcionários-Local-Extras-Marke'!$D43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="31">
-        <v>0</v>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="67">
+        <v>30000</v>
       </c>
       <c r="D44" s="31">
         <v>0</v>
       </c>
       <c r="E44" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C44-'Funcionários-Local-Extras-Marke'!$D44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="31">
-        <v>0</v>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="15"/>
+      <c r="B45" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="67">
+        <v>25000</v>
       </c>
       <c r="D45" s="31">
         <v>0</v>
       </c>
       <c r="E45" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C45-'Funcionários-Local-Extras-Marke'!$D45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="30" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C46" s="31">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D46" s="31">
         <v>0</v>
       </c>
       <c r="E46" s="32">
         <f>'Funcionários-Local-Extras-Marke'!$C46-'Funcionários-Local-Extras-Marke'!$D46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="31">
-        <v>0</v>
-      </c>
-      <c r="D47" s="31">
-        <v>0</v>
-      </c>
-      <c r="E47" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C47-'Funcionários-Local-Extras-Marke'!$D47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" s="31">
-        <v>0</v>
-      </c>
-      <c r="D48" s="31">
-        <v>0</v>
-      </c>
-      <c r="E48" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C48-'Funcionários-Local-Extras-Marke'!$D48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" s="31">
-        <v>0</v>
-      </c>
-      <c r="D49" s="31">
-        <v>0</v>
-      </c>
-      <c r="E49" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C49-'Funcionários-Local-Extras-Marke'!$D49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="31">
-        <v>0</v>
-      </c>
-      <c r="D50" s="31">
-        <v>0</v>
-      </c>
-      <c r="E50" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C50-'Funcionários-Local-Extras-Marke'!$D50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="31">
-        <v>0</v>
-      </c>
-      <c r="D51" s="31">
-        <v>0</v>
-      </c>
-      <c r="E51" s="32">
-        <f>'Funcionários-Local-Extras-Marke'!$C51-'Funcionários-Local-Extras-Marke'!$D51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" s="38">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="73">
         <f>SUBTOTAL(109,Impressão[ESTIMADO])</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="38">
+        <v>120800</v>
+      </c>
+      <c r="D47" s="73">
         <f>SUBTOTAL(109,Impressão[REAL])</f>
         <v>0</v>
       </c>
-      <c r="E52" s="39">
+      <c r="E47" s="34">
         <f>SUBTOTAL(109,Impressão[ACIMA/ABAIXO])</f>
-        <v>0</v>
-      </c>
+        <v>120800</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="80">
+        <f>Impressão[[#Totals],[ESTIMADO]]+Música[[#Totals],[ESTIMADO]]+Festa[[#Totals],[ESTIMADO ANUAL]]+Roupas[[#Totals],[ESTIMADO ANUAL]]</f>
+        <v>1719200</v>
+      </c>
+      <c r="D48" s="38"/>
+      <c r="E48" s="39"/>
+    </row>
+    <row r="49" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="75"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="77"/>
+    </row>
+    <row r="51" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="78">
+        <v>30000000</v>
+      </c>
+      <c r="D52" s="78">
+        <v>0</v>
+      </c>
+      <c r="E52" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C52-'Funcionários-Local-Extras-Marke'!$D52</f>
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="81">
+        <f>C52*8%</f>
+        <v>2400000</v>
+      </c>
+      <c r="D53" s="78">
+        <v>0</v>
+      </c>
+      <c r="E53" s="32">
+        <f>'Funcionários-Local-Extras-Marke'!$C53-'Funcionários-Local-Extras-Marke'!$D53</f>
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="38">
+        <f>C53</f>
+        <v>2400000</v>
+      </c>
+      <c r="D54" s="38">
+        <f>SUBTOTAL(109,Música2[REAL])</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="39">
+        <f>SUBTOTAL(109,Música2[ACIMA/ABAIXO])</f>
+        <v>32400000</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B17:E17"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4175,17 +4375,19 @@
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <tableParts count="4">
-    <tablePart r:id="rId2"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="5">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="158" id="{55199E56-DD9C-4A4F-BED9-16F56CCFDA0D}">
+          <x14:cfRule type="iconSet" priority="162" id="{55199E56-DD9C-4A4F-BED9-16F56CCFDA0D}">
             <x14:iconSet iconSet="3Triangles" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4201,7 +4403,26 @@
               <x14:cfIcon iconSet="3ArrowsGray" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E43:E51 E36:E38 E23:E30 E3:E16</xm:sqref>
+          <xm:sqref>E40:E46 E33:E35 E21:E27 E3:E14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="163" id="{FAF49BCC-35D8-4591-BE60-BF0505A8DFBB}">
+            <x14:iconSet iconSet="3Triangles" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3ArrowsGray" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3ArrowsGray" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E52:E53</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4210,21 +4431,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100438D081558299543A3D90C741E9D9A9A" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="6307e9d03a483d8aaaad55333a2d33a3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4d4739c-b3d2-4350-8f47-3b8a709ccb2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9ddc1d36326b7f09edaeafea200ec074" ns2:_="">
     <xsd:import namespace="a4d4739c-b3d2-4350-8f47-3b8a709ccb2d"/>
@@ -4394,24 +4600,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{953F9F67-1E60-41F1-8D0A-2C9144BB5791}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C15B775D-9D4C-4008-98F9-E820ECDFE507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97900851-B275-4B05-8F5D-F815934E192B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4427,4 +4631,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C15B775D-9D4C-4008-98F9-E820ECDFE507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{953F9F67-1E60-41F1-8D0A-2C9144BB5791}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Planilha de custo atualizada
</commit_message>
<xml_diff>
--- a/Custos para Edição.xlsx
+++ b/Custos para Edição.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Publica\TI0320\Cassio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376D7760-00CA-4850-A8C9-9BEAC1E0241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E49AD05-9291-481D-96C1-DB7E06FE2D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -570,12 +570,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11.5"/>
       <color theme="3"/>
@@ -590,8 +584,15 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,6 +796,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF305353"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9A9A9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -1011,7 +1024,7 @@
     <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1082,7 +1095,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1094,14 +1106,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1134,6 +1144,30 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1159,37 +1193,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="37" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="38" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="38" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Ênfase1" xfId="6" builtinId="30" customBuiltin="1"/>
@@ -1240,9 +1260,104 @@
     <cellStyle name="Total" xfId="5" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="8" builtinId="3" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="62">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <name val="Cambria"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF305353"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <name val="Cambria"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF305353"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <name val="Cambria"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF305353"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <name val="Cambria"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF305353"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="medium">
@@ -1256,6 +1371,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1267,6 +1388,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -1277,6 +1404,12 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1289,7 +1422,22 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="medium">
@@ -1301,23 +1449,29 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1328,25 +1482,22 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="medium">
@@ -1358,11 +1509,29 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1373,7 +1542,21 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="medium">
@@ -1385,11 +1568,29 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1400,7 +1601,41 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <name val="Cambria"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF305353"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="medium">
@@ -1412,11 +1647,29 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1431,9 +1684,6 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1442,14 +1692,26 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
@@ -1723,15 +1985,15 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Orçamento de casamento" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Orçamento de casamento" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="54"/>
-      <tableStyleElement type="headerRow" dxfId="53"/>
-      <tableStyleElement type="totalRow" dxfId="52"/>
-      <tableStyleElement type="lastColumn" dxfId="51"/>
+      <tableStyleElement type="wholeTable" dxfId="61"/>
+      <tableStyleElement type="headerRow" dxfId="60"/>
+      <tableStyleElement type="totalRow" dxfId="59"/>
+      <tableStyleElement type="lastColumn" dxfId="58"/>
     </tableStyle>
     <tableStyle name="Resumo do orçamento de casamento" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="50"/>
-      <tableStyleElement type="headerRow" dxfId="49"/>
-      <tableStyleElement type="totalRow" dxfId="48"/>
+      <tableStyleElement type="wholeTable" dxfId="57"/>
+      <tableStyleElement type="headerRow" dxfId="56"/>
+      <tableStyleElement type="totalRow" dxfId="55"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1801,6 +2063,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF305353"/>
+      <color rgb="FFA9A9A9"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2696,13 +2962,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ResumoDoOrçamento" displayName="ResumoDoOrçamento" ref="C6:F11" totalsRowCount="1" headerRowDxfId="47" totalsRowCellStyle="Total">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ResumoDoOrçamento" displayName="ResumoDoOrçamento" ref="C6:F11" totalsRowCount="1" headerRowDxfId="54" totalsRowCellStyle="Total">
   <autoFilter ref="C6:F10" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CATEGORIA" totalsRowLabel="Total de despesas" totalsRowDxfId="46" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CATEGORIA" totalsRowLabel="Total de despesas" totalsRowDxfId="53" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="48" totalsRowDxfId="47">
       <calculatedColumnFormula>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2716,7 +2982,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Roupas" displayName="Roupas" ref="B2:E15" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Roupas" displayName="Roupas" ref="B2:E15" totalsRowCount="1" headerRowDxfId="24" totalsRowDxfId="25">
   <autoFilter ref="B2:E14" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2724,10 +2990,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Custo¹" dataDxfId="39" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ESTIMADO ANUAL" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="13">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Custo¹" dataDxfId="46" totalsRowDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ESTIMADO ANUAL" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="26">
       <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C3-'Funcionários-Local-Extras-Marke'!$D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2741,7 +3007,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Festa" displayName="Festa" ref="B20:E28" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Festa" displayName="Festa" ref="B20:E28" totalsRowCount="1" headerRowDxfId="3" totalsRowDxfId="19">
   <autoFilter ref="B20:E27" xr:uid="{00000000-0009-0000-0100-00000D000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2749,10 +3015,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Custo" dataDxfId="35" totalsRowDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="ESTIMADO ANUAL" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Custo" dataDxfId="42" totalsRowDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="ESTIMADO ANUAL" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="20">
       <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C21-'Funcionários-Local-Extras-Marke'!$D21</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2766,7 +3032,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Música" displayName="Música" ref="B32:E36" totalsRowCount="1" totalsRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Música" displayName="Música" ref="B32:E36" totalsRowCount="1" headerRowDxfId="2" totalsRowDxfId="14">
   <autoFilter ref="B32:E35" xr:uid="{00000000-0009-0000-0100-00000E000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2774,10 +3040,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Gastos Extras" dataDxfId="30" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="17">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Gastos Extras" dataDxfId="38" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ESTIMADO" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="15">
       <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C33-'Funcionários-Local-Extras-Marke'!$D33</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2791,12 +3057,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Impressão" displayName="Impressão" ref="B39:E47" totalsRowCount="1" totalsRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Impressão" displayName="Impressão" ref="B39:E47" totalsRowCount="1" headerRowDxfId="1" totalsRowDxfId="9">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Marketing" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="ESTIMADO" totalsRowFunction="sum" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" totalsRowDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="CATEGORIA" totalsRowLabel="Total de Marketing" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="ESTIMADO" totalsRowFunction="sum" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="REAL" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="ACIMA/ABAIXO" totalsRowFunction="sum" totalsRowDxfId="10">
       <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C40-'Funcionários-Local-Extras-Marke'!$D40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2810,15 +3076,15 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{542CD9DA-BE67-4476-B3ED-94AAA93D6D50}" name="Música2" displayName="Música2" ref="B51:E54" totalsRowCount="1" totalsRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{542CD9DA-BE67-4476-B3ED-94AAA93D6D50}" name="Música2" displayName="Música2" ref="B51:E54" totalsRowCount="1" headerRowDxfId="0" totalsRowDxfId="4">
   <autoFilter ref="B51:E53" xr:uid="{542CD9DA-BE67-4476-B3ED-94AAA93D6D50}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F828AF69-2C3D-4F7C-BAEB-AE441072E02C}" name="CATEGORIA" totalsRowLabel="Total de Ganho" dataDxfId="11" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{49218F16-1EAB-4FE3-85CD-202EE002DE31}" name="ESTIMADO" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="2">
+    <tableColumn id="1" xr3:uid="{F828AF69-2C3D-4F7C-BAEB-AE441072E02C}" name="CATEGORIA" totalsRowLabel="Total de Ganho" dataDxfId="33" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{49218F16-1EAB-4FE3-85CD-202EE002DE31}" name="ESTIMADO" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="7">
       <totalsRowFormula>C53</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B924C15A-4FC9-4943-9D4C-3A0A2C03CA14}" name="REAL" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{6A452F63-ECF6-47C3-9821-65724FEBC5DB}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0">
+    <tableColumn id="3" xr3:uid="{B924C15A-4FC9-4943-9D4C-3A0A2C03CA14}" name="REAL" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{6A452F63-ECF6-47C3-9821-65724FEBC5DB}" name="ACIMA/ABAIXO" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="5">
       <calculatedColumnFormula>'Funcionários-Local-Extras-Marke'!$C52-'Funcionários-Local-Extras-Marke'!$D52</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3157,30 +3423,30 @@
         <v>3</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3188,16 +3454,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="40" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="3"/>
@@ -3205,18 +3471,18 @@
     <row r="7" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="46">
         <f>Total_de_Roupas_est</f>
         <v>1218000</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="46">
         <f>Total_de_Roupas_real</f>
         <v>0</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="42">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
         <v>1218000</v>
       </c>
@@ -3224,18 +3490,18 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="49">
+      <c r="D8" s="46">
         <f>Total_da_Festa_est</f>
         <v>67900</v>
       </c>
-      <c r="E8" s="49">
+      <c r="E8" s="46">
         <f>Total_da_Festa_real</f>
         <v>0</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="42">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
         <v>67900</v>
       </c>
@@ -3243,18 +3509,18 @@
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="46">
         <f>Total_de_Música_entretenimento_est</f>
         <v>312500</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="46">
         <f>Total_de_Música_entretenimento_real</f>
         <v>0</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="42">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
         <v>312500</v>
       </c>
@@ -3262,18 +3528,18 @@
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="46">
         <f>Total_de_Impressão_gráfica_est</f>
         <v>120800</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="46">
         <f>Total_de_Impressão_gráfica_real</f>
         <v>0</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="42">
         <f>ResumoDoOrçamento[[#This Row],[ESTIMADO]]-ResumoDoOrçamento[[#This Row],[REAL]]</f>
         <v>120800</v>
       </c>
@@ -3281,18 +3547,18 @@
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="47">
         <f>SUBTOTAL(109,ResumoDoOrçamento[ESTIMADO])</f>
         <v>1719200</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="48">
         <f>SUBTOTAL(109,ResumoDoOrçamento[REAL])</f>
         <v>0</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="44">
         <f>SUBTOTAL(109,ResumoDoOrçamento[ACIMA/ABAIXO])</f>
         <v>1719200</v>
       </c>
@@ -3311,204 +3577,204 @@
         <v>15</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
       <c r="G21" s="21"/>
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
       <c r="G29" s="21"/>
     </row>
     <row r="30" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3577,8 +3843,8 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3611,16 +3877,16 @@
       <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="81" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
@@ -3628,738 +3894,738 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <v>120000</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="30">
         <v>0</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C3-'Funcionários-Local-Extras-Marke'!$D3</f>
         <v>120000</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>120000</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <v>0</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C4-'Funcionários-Local-Extras-Marke'!$D4</f>
         <v>120000</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>120000</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="30">
         <v>0</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C5-'Funcionários-Local-Extras-Marke'!$D5</f>
         <v>120000</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>120000</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="30">
         <v>0</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C6-'Funcionários-Local-Extras-Marke'!$D6</f>
         <v>120000</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>120000</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="30">
         <v>0</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C7-'Funcionários-Local-Extras-Marke'!$D7</f>
         <v>120000</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>150000</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="30">
         <v>0</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C8-'Funcionários-Local-Extras-Marke'!$D8</f>
         <v>150000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>108000</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="30">
         <v>0</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C9-'Funcionários-Local-Extras-Marke'!$D9</f>
         <v>108000</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="30">
         <v>108000</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <v>0</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C10-'Funcionários-Local-Extras-Marke'!$D10</f>
         <v>108000</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>108000</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="30">
         <v>0</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C11-'Funcionários-Local-Extras-Marke'!$D11</f>
         <v>108000</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="30">
         <v>72000</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <v>0</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C12-'Funcionários-Local-Extras-Marke'!$D12</f>
         <v>72000</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="30">
         <v>72000</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="30">
         <v>0</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C13-'Funcionários-Local-Extras-Marke'!$D13</f>
         <v>72000</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="30">
         <v>0</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="30">
         <v>0</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C14-'Funcionários-Local-Extras-Marke'!$D14</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="77">
         <f>SUBTOTAL(109,Roupas[ESTIMADO ANUAL])</f>
         <v>1218000</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="77">
         <f>SUBTOTAL(109,Roupas[REAL])</f>
         <v>0</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="78">
         <f>SUBTOTAL(109,Roupas[ACIMA/ABAIXO])</f>
         <v>1218000</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="69"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="57"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="41"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="E19" s="29"/>
+      <c r="C19" s="34"/>
+      <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="87" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="30">
         <v>3000</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="30">
         <v>0</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C21-'Funcionários-Local-Extras-Marke'!$D21</f>
         <v>3000</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="30">
         <v>1500</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="30">
         <v>0</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C22-'Funcionários-Local-Extras-Marke'!$D22</f>
         <v>1500</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="30">
         <v>2400</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="30">
         <v>0</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C23-'Funcionários-Local-Extras-Marke'!$D23</f>
         <v>2400</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="30">
         <v>500</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="30">
         <v>0</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C24-'Funcionários-Local-Extras-Marke'!$D24</f>
         <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="31">
+      <c r="C25" s="30">
         <v>60000</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="30">
         <v>0</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C25-'Funcionários-Local-Extras-Marke'!$D25</f>
         <v>60000</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="31">
+      <c r="C26" s="30">
         <v>0</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="30">
         <v>0</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C26-'Funcionários-Local-Extras-Marke'!$D26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="31">
+      <c r="C27" s="30">
         <v>500</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="30">
         <v>0</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C27-'Funcionários-Local-Extras-Marke'!$D27</f>
         <v>500</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="33">
+      <c r="C28" s="77">
         <f>SUBTOTAL(109,Festa[ESTIMADO ANUAL])</f>
         <v>67900</v>
       </c>
-      <c r="D28" s="33">
+      <c r="D28" s="77">
         <f>SUBTOTAL(109,Festa[REAL])</f>
         <v>0</v>
       </c>
-      <c r="E28" s="34">
+      <c r="E28" s="78">
         <f>SUBTOTAL(109,Festa[ACIMA/ABAIXO])</f>
         <v>67900</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="66"/>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="61"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="63"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="72"/>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="E31" s="29"/>
+      <c r="C31" s="34"/>
+      <c r="E31" s="28"/>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="87" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="31">
+      <c r="C33" s="30">
         <v>0</v>
       </c>
-      <c r="D33" s="31">
+      <c r="D33" s="30">
         <v>0</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C33-'Funcionários-Local-Extras-Marke'!$D33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="67">
+      <c r="C34" s="50">
         <f>625000/2</f>
         <v>312500</v>
       </c>
-      <c r="D34" s="31">
+      <c r="D34" s="30">
         <v>0</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C34-'Funcionários-Local-Extras-Marke'!$D34</f>
         <v>312500</v>
       </c>
-      <c r="G34" s="68">
+      <c r="G34" s="51">
         <v>130000</v>
       </c>
-      <c r="H34" s="68">
+      <c r="H34" s="51">
         <v>45000</v>
       </c>
-      <c r="I34" s="68">
+      <c r="I34" s="51">
         <v>440000</v>
       </c>
-      <c r="J34" s="69">
+      <c r="J34" s="52">
         <v>10000</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="31">
+      <c r="C35" s="30">
         <v>0</v>
       </c>
-      <c r="D35" s="31">
+      <c r="D35" s="30">
         <v>0</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C35-'Funcionários-Local-Extras-Marke'!$D35</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="33">
+      <c r="C36" s="77">
         <f>SUBTOTAL(109,Música[ESTIMADO])</f>
         <v>312500</v>
       </c>
-      <c r="D36" s="33">
+      <c r="D36" s="77">
         <f>SUBTOTAL(109,Música[REAL])</f>
         <v>0</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="78">
         <f>SUBTOTAL(109,Música[ACIMA/ABAIXO])</f>
         <v>312500</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="64"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="66"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="75"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="E38" s="29"/>
+      <c r="C38" s="34"/>
+      <c r="E38" s="28"/>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="29" t="s">
+      <c r="E39" s="87" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="67">
+      <c r="C40" s="50">
         <v>5000</v>
       </c>
-      <c r="D40" s="31">
+      <c r="D40" s="30">
         <v>0</v>
       </c>
-      <c r="E40" s="32">
+      <c r="E40" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C40-'Funcionários-Local-Extras-Marke'!$D40</f>
         <v>5000</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="31">
+      <c r="C41" s="30">
         <v>5000</v>
       </c>
-      <c r="D41" s="31">
+      <c r="D41" s="30">
         <v>0</v>
       </c>
-      <c r="E41" s="32">
+      <c r="E41" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C41-'Funcionários-Local-Extras-Marke'!$D41</f>
         <v>5000</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="31">
+      <c r="C42" s="30">
         <v>5000</v>
       </c>
-      <c r="D42" s="31">
+      <c r="D42" s="30">
         <v>0</v>
       </c>
-      <c r="E42" s="32">
+      <c r="E42" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C42-'Funcionários-Local-Extras-Marke'!$D42</f>
         <v>5000</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="31">
+      <c r="C43" s="30">
         <v>800</v>
       </c>
-      <c r="D43" s="31">
+      <c r="D43" s="30">
         <v>0</v>
       </c>
-      <c r="E43" s="32">
+      <c r="E43" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C43-'Funcionários-Local-Extras-Marke'!$D43</f>
         <v>800</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="67">
+      <c r="C44" s="50">
         <v>30000</v>
       </c>
-      <c r="D44" s="31">
+      <c r="D44" s="30">
         <v>0</v>
       </c>
-      <c r="E44" s="32">
+      <c r="E44" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C44-'Funcionários-Local-Extras-Marke'!$D44</f>
         <v>30000</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15"/>
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="67">
+      <c r="C45" s="50">
         <v>25000</v>
       </c>
-      <c r="D45" s="31">
+      <c r="D45" s="30">
         <v>0</v>
       </c>
-      <c r="E45" s="32">
+      <c r="E45" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C45-'Funcionários-Local-Extras-Marke'!$D45</f>
         <v>25000</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="31">
+      <c r="C46" s="30">
         <v>50000</v>
       </c>
-      <c r="D46" s="31">
+      <c r="D46" s="30">
         <v>0</v>
       </c>
-      <c r="E46" s="32">
+      <c r="E46" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C46-'Funcionários-Local-Extras-Marke'!$D46</f>
         <v>50000</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="73">
+      <c r="C47" s="82">
         <f>SUBTOTAL(109,Impressão[ESTIMADO])</f>
         <v>120800</v>
       </c>
-      <c r="D47" s="73">
+      <c r="D47" s="82">
         <f>SUBTOTAL(109,Impressão[REAL])</f>
         <v>0</v>
       </c>
-      <c r="E47" s="34">
+      <c r="E47" s="78">
         <f>SUBTOTAL(109,Impressão[ACIMA/ABAIXO])</f>
         <v>120800</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="79" t="s">
+      <c r="B48" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="80">
+      <c r="C48" s="60">
         <f>Impressão[[#Totals],[ESTIMADO]]+Música[[#Totals],[ESTIMADO]]+Festa[[#Totals],[ESTIMADO ANUAL]]+Roupas[[#Totals],[ESTIMADO ANUAL]]</f>
         <v>1719200</v>
       </c>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="36"/>
     </row>
     <row r="49" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="74" t="s">
+      <c r="B50" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="75"/>
-      <c r="D50" s="76"/>
-      <c r="E50" s="77"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="57"/>
     </row>
     <row r="51" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="44" t="s">
+      <c r="C51" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="44" t="s">
+      <c r="D51" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="29" t="s">
+      <c r="E51" s="87" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="78">
+      <c r="C52" s="58">
         <v>30000000</v>
       </c>
-      <c r="D52" s="78">
+      <c r="D52" s="58">
         <v>0</v>
       </c>
-      <c r="E52" s="32">
+      <c r="E52" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C52-'Funcionários-Local-Extras-Marke'!$D52</f>
         <v>30000000</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C53" s="81">
+      <c r="C53" s="61">
         <f>C52*8%</f>
         <v>2400000</v>
       </c>
-      <c r="D53" s="78">
+      <c r="D53" s="58">
         <v>0</v>
       </c>
-      <c r="E53" s="32">
+      <c r="E53" s="31">
         <f>'Funcionários-Local-Extras-Marke'!$C53-'Funcionários-Local-Extras-Marke'!$D53</f>
         <v>2400000</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="38">
+      <c r="C54" s="84">
         <f>C53</f>
         <v>2400000</v>
       </c>
-      <c r="D54" s="38">
+      <c r="D54" s="84">
         <f>SUBTOTAL(109,Música2[REAL])</f>
         <v>0</v>
       </c>
-      <c r="E54" s="39">
+      <c r="E54" s="85">
         <f>SUBTOTAL(109,Música2[ACIMA/ABAIXO])</f>
         <v>32400000</v>
       </c>
     </row>
     <row r="55" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C55" s="33"/>
+      <c r="C55" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4431,6 +4697,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100438D081558299543A3D90C741E9D9A9A" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="6307e9d03a483d8aaaad55333a2d33a3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4d4739c-b3d2-4350-8f47-3b8a709ccb2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9ddc1d36326b7f09edaeafea200ec074" ns2:_="">
     <xsd:import namespace="a4d4739c-b3d2-4350-8f47-3b8a709ccb2d"/>
@@ -4600,22 +4881,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{953F9F67-1E60-41F1-8D0A-2C9144BB5791}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C15B775D-9D4C-4008-98F9-E820ECDFE507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97900851-B275-4B05-8F5D-F815934E192B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4631,21 +4914,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C15B775D-9D4C-4008-98F9-E820ECDFE507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{953F9F67-1E60-41F1-8D0A-2C9144BB5791}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Anotações na aba de OBS
</commit_message>
<xml_diff>
--- a/Custos para Edição.xlsx
+++ b/Custos para Edição.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cássio\Documents\SENAC\PROJETO_INTTEGRADOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Publica\TI0320\Cassio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD7C884-A179-44A6-A5A7-D9BE52E0CC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62B9EC16-7C0B-4051-BD8F-CA1485575C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionários-Local-Extras-Marke" sheetId="2" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -313,6 +313,24 @@
   </si>
   <si>
     <t>Escritório</t>
+  </si>
+  <si>
+    <t>Valores correspondente aos gastos com os funcionários (Salário &amp; Encargos)</t>
+  </si>
+  <si>
+    <t>Valores correspondente aos gastos do edifício &amp; material de escritório &amp; Seguro predial</t>
+  </si>
+  <si>
+    <t>Valores corespondente aos veículos (Taxa de importação &amp; traslado &amp; Seguro &amp; Documentação)</t>
+  </si>
+  <si>
+    <t>Valores correspondente a divulgação da marca (empresa)</t>
+  </si>
+  <si>
+    <t>Valor estimado para venda anual</t>
+  </si>
+  <si>
+    <t>Valor que se basea em lucro para efetivar o PPR</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1200,7 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1313,6 +1331,15 @@
     <xf numFmtId="10" fontId="37" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="37" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="37" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1332,13 +1359,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1350,31 +1377,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Ênfase1" xfId="6" builtinId="30" customBuiltin="1"/>
@@ -3879,7 +3907,7 @@
     <col min="2" max="2" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="104" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="80" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -3937,7 +3965,7 @@
         <f>'Funcionários-Local-Extras-Marke'!$C3-'Funcionários-Local-Extras-Marke'!$D3</f>
         <v>119999.90150000001</v>
       </c>
-      <c r="G3" s="105">
+      <c r="G3" s="81">
         <v>0.66500000000000004</v>
       </c>
     </row>
@@ -4110,21 +4138,21 @@
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="85"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="94"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="82"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="91"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
@@ -4174,7 +4202,7 @@
         <f>'Funcionários-Local-Extras-Marke'!$C20-'Funcionários-Local-Extras-Marke'!$D20</f>
         <v>2999.9659999999999</v>
       </c>
-      <c r="G20" s="105">
+      <c r="G20" s="81">
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
@@ -4284,18 +4312,18 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="80" t="s">
+      <c r="B28" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="82"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="91"/>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="86"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="88"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="97"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -4339,20 +4367,20 @@
         <f>'Funcionários-Local-Extras-Marke'!$C32-'Funcionários-Local-Extras-Marke'!$D32</f>
         <v>60000</v>
       </c>
-      <c r="G32" s="105">
+      <c r="G32" s="81">
         <v>0.2215</v>
       </c>
-      <c r="K32" s="108">
+      <c r="K32" s="84">
         <v>0.17499999999999999</v>
       </c>
-      <c r="L32" s="109">
+      <c r="L32" s="85">
         <v>2000000</v>
       </c>
-      <c r="M32" s="110">
+      <c r="M32" s="86">
         <f>L32*K32</f>
         <v>350000</v>
       </c>
-      <c r="N32" s="107"/>
+      <c r="N32" s="83"/>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="13" t="s">
@@ -4369,16 +4397,16 @@
         <f>'Funcionários-Local-Extras-Marke'!$C33-'Funcionários-Local-Extras-Marke'!$D33</f>
         <v>312500</v>
       </c>
-      <c r="K33" s="109">
+      <c r="K33" s="85">
         <v>130000</v>
       </c>
-      <c r="L33" s="109">
+      <c r="L33" s="85">
         <v>45000</v>
       </c>
-      <c r="M33" s="109">
+      <c r="M33" s="85">
         <v>440000</v>
       </c>
-      <c r="N33" s="111">
+      <c r="N33" s="87">
         <v>10000</v>
       </c>
     </row>
@@ -4412,10 +4440,10 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="89"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="91"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="100"/>
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -4458,7 +4486,7 @@
         <f>'Funcionários-Local-Extras-Marke'!$C39-'Funcionários-Local-Extras-Marke'!$D39</f>
         <v>4999.9584999999997</v>
       </c>
-      <c r="G39" s="105">
+      <c r="G39" s="81">
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
@@ -4566,7 +4594,7 @@
         <f>SUBTOTAL(109,Impressão[ACIMA/ABAIXO])</f>
         <v>120799.00140000001</v>
       </c>
-      <c r="G46" s="106">
+      <c r="G46" s="82">
         <f>SUM(G3+G20+G32+G39)</f>
         <v>1</v>
       </c>
@@ -4802,10 +4830,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E16DBF3-7F69-4F61-9D3E-EFC2AAD82ED6}">
-  <dimension ref="B2:M44"/>
+  <dimension ref="A2:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J43" sqref="J43:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4819,7 +4847,9 @@
     <col min="7" max="7" width="12.28515625" style="53" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="53"/>
     <col min="10" max="10" width="4.42578125" style="53" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="53"/>
+    <col min="11" max="12" width="9.140625" style="53"/>
+    <col min="13" max="13" width="17.140625" style="53" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
@@ -4854,24 +4884,24 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="95" t="s">
+    <row r="34" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="96"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="96"/>
-      <c r="K35" s="96"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="97"/>
-    </row>
-    <row r="36" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="105"/>
+      <c r="D35" s="105"/>
+      <c r="E35" s="105"/>
+      <c r="F35" s="105"/>
+      <c r="G35" s="105"/>
+      <c r="H35" s="105"/>
+      <c r="I35" s="105"/>
+      <c r="J35" s="105"/>
+      <c r="K35" s="105"/>
+      <c r="L35" s="105"/>
+      <c r="M35" s="106"/>
+    </row>
+    <row r="36" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="67" t="s">
         <v>0</v>
       </c>
@@ -4893,7 +4923,8 @@
       <c r="L36" s="69"/>
       <c r="M36" s="70"/>
     </row>
-    <row r="37" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="88"/>
       <c r="B37" s="71" t="str">
         <f>'Funcionários-Local-Extras-Marke'!B1</f>
         <v>Funcionários</v>
@@ -4911,12 +4942,14 @@
       </c>
       <c r="H37" s="57"/>
       <c r="I37" s="57"/>
-      <c r="J37" s="98"/>
-      <c r="K37" s="99"/>
-      <c r="L37" s="99"/>
-      <c r="M37" s="100"/>
-    </row>
-    <row r="38" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J37" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="108"/>
+      <c r="L37" s="108"/>
+      <c r="M37" s="109"/>
+    </row>
+    <row r="38" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="72" t="str">
         <f>'Funcionários-Local-Extras-Marke'!B18</f>
         <v>Local Físico*</v>
@@ -4934,12 +4967,14 @@
       </c>
       <c r="H38" s="57"/>
       <c r="I38" s="57"/>
-      <c r="J38" s="101"/>
-      <c r="K38" s="102"/>
-      <c r="L38" s="102"/>
-      <c r="M38" s="103"/>
-    </row>
-    <row r="39" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J38" s="110" t="s">
+        <v>69</v>
+      </c>
+      <c r="K38" s="111"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="112"/>
+    </row>
+    <row r="39" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="72" t="str">
         <f>'Funcionários-Local-Extras-Marke'!B30</f>
         <v>Gastos com Veículos</v>
@@ -4957,12 +4992,14 @@
       </c>
       <c r="H39" s="57"/>
       <c r="I39" s="57"/>
-      <c r="J39" s="101"/>
-      <c r="K39" s="102"/>
-      <c r="L39" s="102"/>
-      <c r="M39" s="103"/>
-    </row>
-    <row r="40" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="110" t="s">
+        <v>70</v>
+      </c>
+      <c r="K39" s="111"/>
+      <c r="L39" s="111"/>
+      <c r="M39" s="112"/>
+    </row>
+    <row r="40" spans="1:13" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="73" t="str">
         <f>'Funcionários-Local-Extras-Marke'!B37</f>
         <v>Marketing</v>
@@ -4980,12 +5017,14 @@
       </c>
       <c r="H40" s="57"/>
       <c r="I40" s="57"/>
-      <c r="J40" s="92"/>
-      <c r="K40" s="93"/>
-      <c r="L40" s="93"/>
-      <c r="M40" s="94"/>
-    </row>
-    <row r="41" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J40" s="101" t="s">
+        <v>71</v>
+      </c>
+      <c r="K40" s="102"/>
+      <c r="L40" s="102"/>
+      <c r="M40" s="103"/>
+    </row>
+    <row r="41" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="58" t="s">
         <v>62</v>
       </c>
@@ -5007,7 +5046,7 @@
       <c r="L41" s="62"/>
       <c r="M41" s="63"/>
     </row>
-    <row r="42" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="56"/>
       <c r="C42" s="57"/>
       <c r="D42" s="57"/>
@@ -5021,7 +5060,7 @@
       <c r="L42" s="57"/>
       <c r="M42" s="64"/>
     </row>
-    <row r="43" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="71" t="s">
         <v>66</v>
       </c>
@@ -5035,12 +5074,14 @@
       <c r="G43" s="65"/>
       <c r="H43" s="65"/>
       <c r="I43" s="65"/>
-      <c r="J43" s="98"/>
-      <c r="K43" s="99"/>
-      <c r="L43" s="99"/>
-      <c r="M43" s="100"/>
-    </row>
-    <row r="44" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J43" s="113" t="s">
+        <v>72</v>
+      </c>
+      <c r="K43" s="114"/>
+      <c r="L43" s="114"/>
+      <c r="M43" s="115"/>
+    </row>
+    <row r="44" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="73" t="str">
         <f>'Funcionários-Local-Extras-Marke'!B55</f>
         <v>PPR</v>
@@ -5055,10 +5096,12 @@
       <c r="G44" s="66"/>
       <c r="H44" s="66"/>
       <c r="I44" s="66"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="93"/>
-      <c r="L44" s="93"/>
-      <c r="M44" s="94"/>
+      <c r="J44" s="101" t="s">
+        <v>73</v>
+      </c>
+      <c r="K44" s="102"/>
+      <c r="L44" s="102"/>
+      <c r="M44" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5071,7 +5114,8 @@
     <mergeCell ref="J43:M43"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5085,6 +5129,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100438D081558299543A3D90C741E9D9A9A" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="6307e9d03a483d8aaaad55333a2d33a3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4d4739c-b3d2-4350-8f47-3b8a709ccb2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9ddc1d36326b7f09edaeafea200ec074" ns2:_="">
     <xsd:import namespace="a4d4739c-b3d2-4350-8f47-3b8a709ccb2d"/>
@@ -5254,12 +5304,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{953F9F67-1E60-41F1-8D0A-2C9144BB5791}">
   <ds:schemaRefs>
@@ -5269,6 +5313,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C15B775D-9D4C-4008-98F9-E820ECDFE507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97900851-B275-4B05-8F5D-F815934E192B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5284,13 +5337,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C15B775D-9D4C-4008-98F9-E820ECDFE507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>